<commit_message>
Results updated in this folder for prompting architecture version002 (iterative, 2-step process) with all images from the images folder
</commit_message>
<xml_diff>
--- a/notebooks/equation extraction development/extraction error check/string mismatch check/extracted_eqs_all versions_EXCEL.xlsx
+++ b/notebooks/equation extraction development/extraction error check/string mismatch check/extracted_eqs_all versions_EXCEL.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,7 +470,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -488,7 +492,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -506,7 +514,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -528,7 +540,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: name 'N' is not defined...</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -549,7 +565,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: name 'l_a' is not defined...</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -567,7 +587,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: can't multiply sequence by non-int of type 'Q'...</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -660,7 +684,11 @@
 ]</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -671,14 +699,215 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>odes = [
-    sympy.Eq(S(t).diff(t), - beta_c * (alpha * A(t) + I(t)) / (Nh - ID_param) * S(t)),
-    sympy.Eq(E(t).diff(t), beta_c * (alpha * A(t) + I(t)) / (Nh - ID_param) * S(t) - sigma * E(t)),
-    sympy.Eq(A(t).diff(t), nu * sigma * E(t) - (theta + gamma_a) * A(t)),
-    sympy.Eq(I(t).diff(t), (1 - nu) * sigma * E(t) - (psi + gamma_O + dO) * I(t)),
-    sympy.Eq(ID(t).diff(t), theta * A(t) + psi * I(t) - (gamma_i + dD) * ID(t)),
-    sympy.Eq(R(t).diff(t), gamma_i * ID(t) + gamma_a * A(t) + gamma_O * I(t))
-]</t>
+          <t>FAILED: Error while executing the code: 'Symbol' object is not callable...</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>BIOMD0000000964</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>BIOMD0000000970</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BIOMD0000000974</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BIOMD0000000963</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>BIOMD0000000977</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>odes_to_mira_SEVITHR</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BIOMD0000000984</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BIOMD0000000978</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Dec_2024_epi_scenario1_modelC</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Dec_2024_epi_scenario1_modelB</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>SUCCESS - No ODE string stored</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BIOMD0000000972</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: 'Symbol' object is not callable...</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BIOMD0000000971</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: name 'theta' is not defined...</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BIOMD0000000976</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: 'Symbol' object is not callable...</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BIOMD0000000979</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: exec() arg 1 must be a string, bytes or code object...</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BIOMD0000000983</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: 'Symbol' object is not callable...</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Dec_2024_epi_scenario1_modelA</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>FAILED: Error while executing the code: name 'pi_n' is not defined...</t>
         </is>
       </c>
     </row>

</xml_diff>